<commit_message>
commit with import drugs from pdf
</commit_message>
<xml_diff>
--- a/drugs_list1.xlsx
+++ b/drugs_list1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Index</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Adrenaline</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>Contraceptives Overview</t>
   </si>
   <si>
+    <t>Crocin</t>
+  </si>
+  <si>
     <t>Dexamethasone</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t>Dicloxacillin</t>
   </si>
   <si>
+    <t>Dolo</t>
+  </si>
+  <si>
     <t>Ergometrine</t>
   </si>
   <si>
@@ -103,6 +112,9 @@
     <t>Hydralazine</t>
   </si>
   <si>
+    <t>Ibujesic</t>
+  </si>
+  <si>
     <t>Ibuprofen</t>
   </si>
   <si>
@@ -191,6 +203,9 @@
   </si>
   <si>
     <t>Vitamin X</t>
+  </si>
+  <si>
+    <t>item.str</t>
   </si>
 </sst>
 </file>
@@ -567,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B66"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -755,7 +770,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -763,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -771,7 +786,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +794,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +802,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +810,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +818,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +826,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +834,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +842,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +850,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +858,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +866,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +874,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +882,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +890,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +898,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +906,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +914,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -907,7 +922,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,7 +930,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -923,7 +938,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +946,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +954,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,7 +962,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,7 +970,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,7 +978,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,7 +986,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +994,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +1002,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +1010,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +1018,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1011,7 +1026,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1034,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,7 +1042,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1050,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,7 +1058,63 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>